<commit_message>
Update timesheet by Arul
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet 1 (1).xlsx
+++ b/Process/Timesheet/PTW-Timesheet 1 (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BDA8DFE-859C-4107-A2B3-8A646E4EF1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{374CB735-B4C8-47E0-875A-DECD278D2515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5-4-22" sheetId="40" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="145">
   <si>
     <t>Resource Name</t>
   </si>
@@ -475,6 +475,15 @@
     <t xml:space="preserve">others(lunch &amp; tea break)-1.30hr                        </t>
   </si>
   <si>
+    <t>UI for  trainee and trainer</t>
+  </si>
+  <si>
+    <t>Group discussion about UI integration - 45 mins , Entity modelling - 1 hour,Consistency checking - 2 hours,Meeting with rafi - 1.45 mins</t>
+  </si>
+  <si>
+    <t>Lunch : 1hour, Break:20 mins</t>
+  </si>
+  <si>
     <t>Group discussion about UI integration - 45 mins , Entity modelling - 1 hour,Consistency checking - 2 hours,Session with Rafi - 100 mins</t>
   </si>
   <si>
@@ -485,7 +494,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,6 +582,24 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -618,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -676,6 +703,15 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1017,7 +1053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="B4:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="B12" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1335,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB7CC24-ECCE-4106-96A6-9EE0F697F084}">
   <dimension ref="B4:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1900,8 +1936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7951E731-BC0F-4432-8EF7-5AB4C8202D9B}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>
@@ -2148,56 +2184,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A377B9-DC0C-451C-B12D-A0709E33CEF2}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="45">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="22" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="73.5" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="12" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:8" ht="100.5" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -2206,112 +2242,112 @@
       <c r="C3" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F3" s="12" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>123</v>
       </c>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:8" ht="160.5" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="14" t="s">
         <v>126</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" ht="170.25" customHeight="1">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="13" t="s">
         <v>130</v>
       </c>
       <c r="F5" s="13"/>
-      <c r="G5" s="8"/>
+      <c r="G5" s="24"/>
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" ht="165" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="13" t="s">
         <v>134</v>
       </c>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="85.5" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="12" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="13" t="s">
         <v>137</v>
       </c>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="102.75" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="14" t="s">
         <v>119</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="13" t="s">
         <v>139</v>
       </c>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="191.25" customHeight="1">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -2332,11 +2368,11 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:8" ht="123.75" customHeight="1">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>94</v>
@@ -2353,40 +2389,38 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="164.25" customHeight="1">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>114</v>
+      <c r="C11" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>142</v>
       </c>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="87" customHeight="1">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>141</v>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>144</v>
       </c>
       <c r="G12" s="4"/>
     </row>

</xml_diff>